<commit_message>
finished test_fitness.m, nearly done with test_substances.m
</commit_message>
<xml_diff>
--- a/dice_cov_fitness.xlsx
+++ b/dice_cov_fitness.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leon Tannenbaum\Documents\Texas A&amp;M\Aero 614 - Human Performance in Aerospace Environments\DICE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6DC35D2-9B62-4413-BA7D-075658DA2F70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A542C9-DEAE-49F7-8075-BDACED25CF44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-83" yWindow="-83" windowWidth="28965" windowHeight="15766" activeTab="9" xr2:uid="{480C51D9-5374-4262-BBEB-32D406A0B3EF}"/>
+    <workbookView xWindow="38270" yWindow="70" windowWidth="38660" windowHeight="21260" activeTab="2" xr2:uid="{480C51D9-5374-4262-BBEB-32D406A0B3EF}"/>
   </bookViews>
   <sheets>
     <sheet name="pos_impact_week_ny" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="time_mpa_mm" sheetId="8" r:id="rId7"/>
     <sheet name="walk_7days_mm" sheetId="9" r:id="rId8"/>
     <sheet name="time_walk_mm" sheetId="10" r:id="rId9"/>
-    <sheet name="Sheet11" sheetId="11" r:id="rId10"/>
+    <sheet name="sitting_7days_mm" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1075,7 +1075,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{163381E3-7F6B-4121-9906-3C288FB312B8}">
   <dimension ref="A2:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
@@ -1705,7 +1705,7 @@
   <dimension ref="A2:L20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2257,8 +2257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4826B0D5-E81F-4E47-8EC8-CCC6D08F1986}">
   <dimension ref="A2:L20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:L20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S47" sqref="S47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>